<commit_message>
fix postgre problem, add summarize copy function
</commit_message>
<xml_diff>
--- a/init.xlsx
+++ b/init.xlsx
@@ -8,22 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pythonCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E6865D-9086-4D25-A717-8BE56D3C7D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E14061C-38D8-4F9E-B7EB-106C1A948C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29700" yWindow="-4760" windowWidth="20330" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-5330" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula" sheetId="2" r:id="rId1"/>
-    <sheet name="Value" sheetId="7" r:id="rId2"/>
-    <sheet name="Special Formula" sheetId="9" r:id="rId3"/>
-    <sheet name="Operator" sheetId="8" r:id="rId4"/>
+    <sheet name="Formula_SqlServer" sheetId="10" r:id="rId2"/>
+    <sheet name="Formula_MySql" sheetId="11" r:id="rId3"/>
+    <sheet name="Formula_Postgre" sheetId="12" r:id="rId4"/>
+    <sheet name="Value" sheetId="7" r:id="rId5"/>
+    <sheet name="Value_Postgre" sheetId="13" r:id="rId6"/>
+    <sheet name="Special Formula" sheetId="9" r:id="rId7"/>
+    <sheet name="Operator" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="102">
   <si>
     <t>Type</t>
   </si>
@@ -587,6 +591,18 @@
     <t>负数的小数次幂，报错</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -599,7 +615,7 @@
     <numFmt numFmtId="179" formatCode="0.00000_ "/>
     <numFmt numFmtId="180" formatCode="0.000000000000000_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,6 +635,12 @@
       <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -675,7 +697,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -755,6 +777,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1034,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1077,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1241,7 +1266,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
@@ -1415,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -1550,11 +1575,258 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78325629-F2D2-40E7-BAD9-98E2AF874394}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="L42" sqref="L42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDBAF02-78FC-4029-B952-86F85A01C338}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="10">
+        <v>3</v>
+      </c>
+      <c r="C2" s="10">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C2EBEA-A628-40E2-9D1E-C75F02B08FEA}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G47" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1564,9 +1836,10 @@
     <col min="3" max="3" width="18.6640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="46.33203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
@@ -1582,8 +1855,11 @@
       <c r="E1" s="25" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -1599,8 +1875,11 @@
       <c r="E2" s="25">
         <v>0.79166666666666663</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
@@ -1616,8 +1895,11 @@
       <c r="E3" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>42</v>
       </c>
@@ -1634,7 +1916,7 @@
         <v>0.1257175925925926</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>68</v>
       </c>
@@ -1648,7 +1930,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>69</v>
       </c>
@@ -1659,7 +1941,7 @@
         <v>1.0000100000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>46</v>
       </c>
@@ -1667,22 +1949,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>74</v>
       </c>
@@ -1694,7 +1976,140 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833837E6-B291-472A-B144-40663CFCA1C9}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="6"/>
+    <col min="2" max="2" width="9" style="2"/>
+    <col min="3" max="3" width="18.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>37641</v>
+      </c>
+      <c r="E2" s="25">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-7</v>
+      </c>
+      <c r="C3" s="7">
+        <v>-2.5</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1830,7 +2245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>

</xml_diff>